<commit_message>
Eliminating duplications in values in reporting sections.
</commit_message>
<xml_diff>
--- a/DMFX.FinRatios.xlsx
+++ b/DMFX.FinRatios.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -144,9 +145,6 @@
     <t>DE</t>
   </si>
   <si>
-    <t xml:space="preserve">TotalLiabilities / TotalShareholdersEquity </t>
-  </si>
-  <si>
     <t>Interest Coverage Ratio</t>
   </si>
   <si>
@@ -249,9 +247,6 @@
     <t>(AssetsCurrent - InventoryNet) / LiabilitiesCurrent</t>
   </si>
   <si>
-    <t>Liabilities / StockholdersEquity</t>
-  </si>
-  <si>
     <t>OperatingIncomeLoss / InterestExpense</t>
   </si>
   <si>
@@ -271,6 +266,24 @@
   </si>
   <si>
     <t>CostOfGoodsAndServicesSold / (  (AccountsPayableCurrent[0] + AccountsPayableCurrent[1])/2 )</t>
+  </si>
+  <si>
+    <t>Financial Leverage</t>
+  </si>
+  <si>
+    <t>FinLev</t>
+  </si>
+  <si>
+    <t>TotalDebt / TotalShareholdersEquity</t>
+  </si>
+  <si>
+    <t>/ StockholdersEquity</t>
+  </si>
+  <si>
+    <t>(LongTermDebtCurrent + LongTermDebtNoncurrent) / StockholdersEquity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(LongTermDebt + ShortTermDebt) / TotalShareholdersEquity </t>
   </si>
 </sst>
 </file>
@@ -699,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H26"/>
+  <dimension ref="B3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,10 +756,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -765,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -782,7 +795,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -799,24 +812,24 @@
         <v>28</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F8" t="s">
-        <v>68</v>
+      <c r="F8" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -833,7 +846,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -850,24 +863,24 @@
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
-        <v>71</v>
+      <c r="F11" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -884,7 +897,7 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
@@ -901,7 +914,7 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -918,7 +931,7 @@
         <v>26</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -935,7 +948,7 @@
         <v>36</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -952,41 +965,41 @@
         <v>39</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" t="s">
-        <v>77</v>
+      <c r="E17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
-        <v>78</v>
+      <c r="F18" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -994,16 +1007,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
         <v>46</v>
       </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -1011,16 +1024,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1028,16 +1041,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1045,16 +1058,16 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" t="s">
-        <v>60</v>
-      </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1062,16 +1075,16 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -1079,16 +1092,16 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
@@ -1096,16 +1109,16 @@
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -1113,16 +1126,33 @@
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding CFTC COT parser
</commit_message>
<xml_diff>
--- a/DMFX.FinRatios.xlsx
+++ b/DMFX.FinRatios.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,104 +1025,104 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
+      <c r="B21" s="12">
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="5">
+      <c r="B22" s="12">
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="3">
+      <c r="B23" s="12">
         <v>19</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="3">
+      <c r="B24" s="12">
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="5">
+      <c r="B25" s="12">
         <v>21</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="3">
+      <c r="B26" s="12">
         <v>22</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="14" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>